<commit_message>
Adding some constraints to the constraints_weightings
</commit_message>
<xml_diff>
--- a/RiskParity_Constraints.xlsx
+++ b/RiskParity_Constraints.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -573,12 +573,35 @@
         <v>&gt;=</v>
       </c>
       <c r="G8" t="str">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Asset</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Class 1</v>
+      </c>
+      <c r="E9" t="str">
+        <v>QQQ</v>
+      </c>
+      <c r="F9" t="str">
+        <v>&gt;</v>
+      </c>
+      <c r="G9" t="str">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more changes to constraints
</commit_message>
<xml_diff>
--- a/RiskParity_Constraints.xlsx
+++ b/RiskParity_Constraints.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -561,7 +561,7 @@
         <v>FALSE</v>
       </c>
       <c r="C8" t="str">
-        <v>Asset</v>
+        <v>Assets</v>
       </c>
       <c r="E8" t="str">
         <v>SPY</v>
@@ -573,7 +573,7 @@
         <v>0.01</v>
       </c>
       <c r="H8" t="str">
-        <v>Asset</v>
+        <v>Assets</v>
       </c>
     </row>
     <row r="9">
@@ -584,7 +584,7 @@
         <v>FALSE</v>
       </c>
       <c r="C9" t="str">
-        <v>Asset</v>
+        <v>Assets</v>
       </c>
       <c r="E9" t="str">
         <v>QQQ</v>
@@ -596,12 +596,29 @@
         <v>0.05</v>
       </c>
       <c r="H9" t="str">
-        <v>Asset</v>
+        <v>Assets</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="C10" t="str">
+        <v>All Assets</v>
+      </c>
+      <c r="F10" t="str">
+        <v>&gt;=</v>
+      </c>
+      <c r="G10" t="str">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More fix to energy 20%
</commit_message>
<xml_diff>
--- a/RiskParity_Constraints.xlsx
+++ b/RiskParity_Constraints.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -523,7 +523,7 @@
         <v>Energies</v>
       </c>
       <c r="F5" t="str">
-        <v>&lt;</v>
+        <v>=&lt;</v>
       </c>
       <c r="G5" t="str">
         <v>0.2</v>
@@ -612,7 +612,7 @@
         <v>QQQ</v>
       </c>
       <c r="F9" t="str">
-        <v>&gt;</v>
+        <v>&gt;=</v>
       </c>
       <c r="G9" t="str">
         <v>0.01</v>
@@ -661,32 +661,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>11</v>
-      </c>
-      <c r="B12" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Assets</v>
-      </c>
-      <c r="E12" t="str">
-        <v>IUES.L</v>
-      </c>
-      <c r="F12" t="str">
-        <v>&lt;</v>
-      </c>
-      <c r="G12" t="str">
-        <v>0.2</v>
-      </c>
-      <c r="H12" t="str">
-        <v>Assets</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>